<commit_message>
Final results of YOLO Detection
</commit_message>
<xml_diff>
--- a/tommaso/yolo/RESULTS YOLO.xlsx
+++ b/tommaso/yolo/RESULTS YOLO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma3-my.sharepoint.com/personal/tom_senatori_stud_uniroma3_it/Documents/Desktop/AI_LUX/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C56CDE44-7B24-4D85-8F2E-421F572B6195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BDD291E-BDA7-4A61-832D-5B30D64F9920}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{C56CDE44-7B24-4D85-8F2E-421F572B6195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE600DA-5FF0-4B21-A988-E9607DF2EA99}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{7B87E533-CA9B-482E-9687-93226B63E52D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{7B87E533-CA9B-482E-9687-93226B63E52D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>YOLO</t>
   </si>
@@ -74,7 +74,19 @@
     <t>11s</t>
   </si>
   <si>
-    <t>RIALLENA</t>
+    <t>RISCRIVI</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>s per epoch</t>
+  </si>
+  <si>
+    <t>heavy</t>
+  </si>
+  <si>
+    <t>11m</t>
   </si>
 </sst>
 </file>
@@ -446,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EDA54E-D0CA-4A0F-B0E9-B84BCEEFA107}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -457,6 +469,7 @@
     <col min="1" max="1" width="9.1328125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="13.53125" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="11.19921875" customWidth="1"/>
   </cols>
@@ -471,6 +484,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
@@ -495,31 +511,32 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2">
+        <f>(F2*3600)/E2</f>
+        <v>11.556000000000001</v>
+      </c>
       <c r="E2">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>3.7999999999999999E-2</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="G2">
-        <v>0.94599999999999995</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="H2">
-        <v>0.93600000000000005</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="I2">
-        <v>0.97299999999999998</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="J2">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
+        <v>0.82899999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -527,28 +544,32 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3">
+        <f>(F3*3600)/E3</f>
+        <v>12.094382022471908</v>
+      </c>
       <c r="E3">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F3">
-        <v>0.19700000000000001</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="G3">
-        <v>0.99199999999999999</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="H3">
-        <v>0.99099999999999999</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="I3">
-        <v>0.995</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="J3">
-        <v>0.93700000000000006</v>
+        <v>0.91800000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -556,28 +577,32 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>640</v>
+        <v>512</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4">
+        <f>(F4*3600)/E4</f>
+        <v>20.759999999999998</v>
+      </c>
       <c r="E4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>0.38800000000000001</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="G4">
-        <v>0.96799999999999997</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="H4">
-        <v>0.96299999999999997</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="I4">
-        <v>0.99199999999999999</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="J4">
-        <v>0.92800000000000005</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
@@ -588,48 +613,56 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>1024</v>
+        <v>640</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="D5">
+        <f>(F5*3600)/E5</f>
+        <v>27.430985915492961</v>
+      </c>
       <c r="E5">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="F5">
-        <v>0.40699999999999997</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="G5">
-        <v>0.98699999999999999</v>
+        <v>0.997</v>
       </c>
       <c r="H5">
-        <v>0.98399999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="I5">
-        <v>0.99299999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="J5">
-        <v>0.93799999999999994</v>
+        <v>0.95399999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
+      <c r="D6">
+        <f>(F6*3600)/E6</f>
+        <v>47.53846153846154</v>
+      </c>
       <c r="E6">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F6">
-        <v>0.39</v>
+        <v>1.03</v>
       </c>
       <c r="G6">
-        <v>0.998</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="H6">
         <v>0.997</v>
@@ -638,7 +671,172 @@
         <v>0.995</v>
       </c>
       <c r="J6">
-        <v>0.96599999999999997</v>
+        <v>0.96199999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>640</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <f>(F7*3600)/E7</f>
+        <v>27.99</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>0.311</v>
+      </c>
+      <c r="G7">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J7">
+        <v>0.95199999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>640</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <f>(F8*3600)/E8</f>
+        <v>25.667999999999996</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="G8">
+        <v>0.997</v>
+      </c>
+      <c r="H8">
+        <v>0.998</v>
+      </c>
+      <c r="I8">
+        <v>0.995</v>
+      </c>
+      <c r="J8">
+        <v>0.96299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>640</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <f>(F9*3600)/E9</f>
+        <v>25.92</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>1.08</v>
+      </c>
+      <c r="G9">
+        <v>0.998</v>
+      </c>
+      <c r="H9">
+        <v>0.999</v>
+      </c>
+      <c r="I9">
+        <v>0.995</v>
+      </c>
+      <c r="J9">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <f>(F10*3600)/E10</f>
+        <v>11.447999999999999</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="H10">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>640</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f>(F11*3600)/E11</f>
+        <v>48.46153846153846</v>
+      </c>
+      <c r="E11">
+        <v>52</v>
+      </c>
+      <c r="F11">
+        <v>0.7</v>
+      </c>
+      <c r="G11">
+        <v>0.99</v>
+      </c>
+      <c r="H11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.95299999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all YOLO files
From dataset generation to training to results to final submission
</commit_message>
<xml_diff>
--- a/tommaso/yolo/RESULTS YOLO.xlsx
+++ b/tommaso/yolo/RESULTS YOLO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma3-my.sharepoint.com/personal/tom_senatori_stud_uniroma3_it/Documents/Desktop/AI_LUX/CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{C56CDE44-7B24-4D85-8F2E-421F572B6195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE600DA-5FF0-4B21-A988-E9607DF2EA99}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{C56CDE44-7B24-4D85-8F2E-421F572B6195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CC40CCB-4205-47AE-A2A1-9168983A977E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{7B87E533-CA9B-482E-9687-93226B63E52D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>YOLO</t>
   </si>
@@ -74,9 +74,6 @@
     <t>11s</t>
   </si>
   <si>
-    <t>RISCRIVI</t>
-  </si>
-  <si>
     <t>light</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>11m</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -122,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EDA54E-D0CA-4A0F-B0E9-B84BCEEFA107}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -474,7 +478,7 @@
     <col min="10" max="10" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -505,12 +509,18 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>128</v>
       </c>
       <c r="C2" t="s">
@@ -539,18 +549,18 @@
         <v>0.82899999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>256</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3">
-        <f>(F3*3600)/E3</f>
+        <f t="shared" ref="D3:D13" si="0">(F3*3600)/E3</f>
         <v>12.094382022471908</v>
       </c>
       <c r="E3">
@@ -572,54 +582,51 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>512</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4">
-        <f>(F4*3600)/E4</f>
-        <v>20.759999999999998</v>
+        <f t="shared" si="0"/>
+        <v>20.252571428571425</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F4">
-        <v>0.17299999999999999</v>
+        <v>0.19689999999999999</v>
       </c>
       <c r="G4">
-        <v>0.98399999999999999</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="H4">
-        <v>0.98699999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="I4">
-        <v>0.99299999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="J4">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>640</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5">
-        <f>(F5*3600)/E5</f>
+        <f t="shared" si="0"/>
         <v>27.430985915492961</v>
       </c>
       <c r="E5">
@@ -640,19 +647,22 @@
       <c r="J5">
         <v>0.95399999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="L5">
+        <v>0.93789999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>1024</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6">
-        <f>(F6*3600)/E6</f>
+        <f t="shared" si="0"/>
         <v>47.53846153846154</v>
       </c>
       <c r="E6">
@@ -674,18 +684,18 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>640</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7">
-        <f>(F7*3600)/E7</f>
+        <f t="shared" si="0"/>
         <v>27.99</v>
       </c>
       <c r="E7">
@@ -707,18 +717,18 @@
         <v>0.95199999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>640</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <f>(F8*3600)/E8</f>
+        <f t="shared" si="0"/>
         <v>25.667999999999996</v>
       </c>
       <c r="E8">
@@ -739,19 +749,22 @@
       <c r="J8">
         <v>0.96299999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="L8">
+        <v>0.94450000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>640</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9">
-        <f>(F9*3600)/E9</f>
+        <f t="shared" si="0"/>
         <v>25.92</v>
       </c>
       <c r="E9">
@@ -773,18 +786,18 @@
         <v>0.96099999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>256</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <f>(F10*3600)/E10</f>
+        <f t="shared" si="0"/>
         <v>11.447999999999999</v>
       </c>
       <c r="E10">
@@ -806,18 +819,18 @@
         <v>0.91800000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
         <v>640</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <f>(F11*3600)/E11</f>
+        <f t="shared" si="0"/>
         <v>48.46153846153846</v>
       </c>
       <c r="E11">
@@ -837,6 +850,78 @@
       </c>
       <c r="J11">
         <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>512</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>23.4</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <v>0.39</v>
+      </c>
+      <c r="G12">
+        <v>0.998</v>
+      </c>
+      <c r="H12">
+        <v>0.997</v>
+      </c>
+      <c r="I12">
+        <v>0.995</v>
+      </c>
+      <c r="J12">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="L12">
+        <v>0.94340000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>640</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>28.91566265060241</v>
+      </c>
+      <c r="E13">
+        <v>249</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>0.997</v>
+      </c>
+      <c r="H13">
+        <v>0.998</v>
+      </c>
+      <c r="I13">
+        <v>0.995</v>
+      </c>
+      <c r="J13">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="L13">
+        <v>0.93689999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>